<commit_message>
Added Active Climate Deniers
</commit_message>
<xml_diff>
--- a/data/Representatives.xlsx
+++ b/data/Representatives.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Govt Climate Denialists\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB458F8-137F-40AB-AE11-D2C136F98A4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F60EA7B-EE9C-4BE2-A284-7978690CA659}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="270" windowWidth="28800" windowHeight="15435" xr2:uid="{62D81309-DA17-4AA3-9DB3-296B4017ED59}"/>
+    <workbookView xWindow="5880" yWindow="1680" windowWidth="28800" windowHeight="15435" xr2:uid="{62D81309-DA17-4AA3-9DB3-296B4017ED59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="373">
   <si>
     <t>Hon Anthony Albanese</t>
   </si>
@@ -1353,6 +1353,15 @@
   </si>
   <si>
     <t>Member of Parliamentary Friends of Climate Action</t>
+  </si>
+  <si>
+    <t>Actively denies climate change in the public sphere</t>
+  </si>
+  <si>
+    <t>Continues to point to debunked and false theories</t>
+  </si>
+  <si>
+    <t>Acknowledges climate change is real but continues to push debunked theories</t>
   </si>
 </sst>
 </file>
@@ -1801,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADEF58E-A175-4784-867D-6B850DC00D7C}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="O114" sqref="O114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2892,13 +2901,16 @@
         <v>19</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="8">
         <v>104915</v>
       </c>
       <c r="H41" t="s">
         <v>358</v>
+      </c>
+      <c r="I41" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3866,13 +3878,16 @@
         <v>19</v>
       </c>
       <c r="F78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78" s="8">
         <v>106096</v>
       </c>
       <c r="H78" t="s">
         <v>358</v>
+      </c>
+      <c r="I78" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4884,13 +4899,16 @@
         <v>342</v>
       </c>
       <c r="F116" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G116" s="8">
         <v>111841</v>
       </c>
       <c r="H116" t="s">
         <v>358</v>
+      </c>
+      <c r="I116" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Changed OneNation to active climate change deniers
</commit_message>
<xml_diff>
--- a/data/Representatives.xlsx
+++ b/data/Representatives.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Govt Climate Denialists\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F60EA7B-EE9C-4BE2-A284-7978690CA659}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A280B0-B29F-4941-9E71-34800F035954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="1680" windowWidth="28800" windowHeight="15435" xr2:uid="{62D81309-DA17-4AA3-9DB3-296B4017ED59}"/>
+    <workbookView xWindow="6225" yWindow="2025" windowWidth="28800" windowHeight="15435" xr2:uid="{62D81309-DA17-4AA3-9DB3-296B4017ED59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="374">
   <si>
     <t>Hon Anthony Albanese</t>
   </si>
@@ -1362,6 +1362,9 @@
   </si>
   <si>
     <t>Acknowledges climate change is real but continues to push debunked theories</t>
+  </si>
+  <si>
+    <t>At the very least, a climate change sceptic, on record as late as Sep 2019 as denying climate change is man made before later "clarifying" his position</t>
   </si>
 </sst>
 </file>
@@ -1810,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADEF58E-A175-4784-867D-6B850DC00D7C}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="O114" sqref="O114"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4556,6 +4559,9 @@
       </c>
       <c r="H103" t="s">
         <v>358</v>
+      </c>
+      <c r="I103" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added additional plots to the resident graph
</commit_message>
<xml_diff>
--- a/data/Representatives.xlsx
+++ b/data/Representatives.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Govt Climate Denialists\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A280B0-B29F-4941-9E71-34800F035954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F1DF10-CA04-4E7A-B4C6-E880BFB46375}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6225" yWindow="2025" windowWidth="28800" windowHeight="15435" xr2:uid="{62D81309-DA17-4AA3-9DB3-296B4017ED59}"/>
+    <workbookView xWindow="40830" yWindow="915" windowWidth="28800" windowHeight="15435" xr2:uid="{62D81309-DA17-4AA3-9DB3-296B4017ED59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$152</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$152</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="375">
   <si>
     <t>Hon Anthony Albanese</t>
   </si>
@@ -1366,11 +1368,17 @@
   <si>
     <t>At the very least, a climate change sceptic, on record as late as Sep 2019 as denying climate change is man made before later "clarifying" his position</t>
   </si>
+  <si>
+    <t>Area SqKm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.000000000000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1468,7 +1476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1496,6 +1504,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1811,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADEF58E-A175-4784-867D-6B850DC00D7C}">
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:J152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="M139" sqref="M139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,10 +1835,11 @@
     <col min="5" max="5" width="40.85546875" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>331</v>
       </c>
@@ -1852,10 +1862,13 @@
         <v>353</v>
       </c>
       <c r="H1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>116</v>
       </c>
@@ -1877,11 +1890,14 @@
       <c r="G2" s="8">
         <v>122050</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="11">
+        <v>86.38</v>
+      </c>
+      <c r="I2" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>296</v>
       </c>
@@ -1903,11 +1919,14 @@
       <c r="G3" s="8">
         <v>111107</v>
       </c>
-      <c r="H3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="11">
+        <v>113.78</v>
+      </c>
+      <c r="I3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>172</v>
       </c>
@@ -1929,11 +1948,14 @@
       <c r="G4" s="8">
         <v>115918</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="11">
+        <v>4322.38</v>
+      </c>
+      <c r="I4" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
@@ -1955,11 +1977,14 @@
       <c r="G5" s="8">
         <v>107182</v>
       </c>
-      <c r="H5" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="11">
+        <v>53.007212355657003</v>
+      </c>
+      <c r="I5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>230</v>
       </c>
@@ -1981,11 +2006,14 @@
       <c r="G6" s="8">
         <v>119110</v>
       </c>
-      <c r="H6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="11">
+        <v>65206.36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
@@ -2007,11 +2035,14 @@
       <c r="G7" s="8">
         <v>109249</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="11">
+        <v>39.608255317976997</v>
+      </c>
+      <c r="I7" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -2033,11 +2064,14 @@
       <c r="G8" s="8">
         <v>76979</v>
       </c>
-      <c r="H8" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="11">
+        <v>7975.9555819632997</v>
+      </c>
+      <c r="I8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>268</v>
       </c>
@@ -2059,14 +2093,17 @@
       <c r="G9" s="8">
         <v>105166</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="11">
+        <v>1913.9697369266</v>
+      </c>
+      <c r="I9" t="s">
         <v>360</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>64</v>
       </c>
@@ -2088,11 +2125,14 @@
       <c r="G10" s="8">
         <v>113527</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="11">
+        <v>5496.5</v>
+      </c>
+      <c r="I10" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -2114,11 +2154,14 @@
       <c r="G11" s="8">
         <v>109661</v>
       </c>
-      <c r="H11" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="11">
+        <v>60.265557340260997</v>
+      </c>
+      <c r="I11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>180</v>
       </c>
@@ -2140,11 +2183,14 @@
       <c r="G12" s="8">
         <v>106369</v>
       </c>
-      <c r="H12" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="11">
+        <v>786.40134002481</v>
+      </c>
+      <c r="I12" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>216</v>
       </c>
@@ -2166,11 +2212,14 @@
       <c r="G13" s="8">
         <v>114650</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="11">
+        <v>6472.0418602978998</v>
+      </c>
+      <c r="I13" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
@@ -2192,11 +2241,14 @@
       <c r="G14" s="8">
         <v>105796</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="11">
+        <v>61.071030977805997</v>
+      </c>
+      <c r="I14" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>302</v>
       </c>
@@ -2218,11 +2270,14 @@
       <c r="G15" s="8">
         <v>105161</v>
       </c>
-      <c r="H15" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="11">
+        <v>371.33719549777999</v>
+      </c>
+      <c r="I15" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>108</v>
       </c>
@@ -2244,11 +2299,14 @@
       <c r="G16" s="8">
         <v>124133</v>
       </c>
-      <c r="H16" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="11">
+        <v>115.62</v>
+      </c>
+      <c r="I16" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>176</v>
       </c>
@@ -2270,11 +2328,14 @@
       <c r="G17" s="8">
         <v>109745</v>
       </c>
-      <c r="H17" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="11">
+        <v>536.30704580510996</v>
+      </c>
+      <c r="I17" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>234</v>
       </c>
@@ -2296,11 +2357,14 @@
       <c r="G18" s="8">
         <v>79557</v>
       </c>
-      <c r="H18" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="11">
+        <v>21369.238841563001</v>
+      </c>
+      <c r="I18" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>105</v>
       </c>
@@ -2322,11 +2386,14 @@
       <c r="G19" s="8">
         <v>107371</v>
       </c>
-      <c r="H19" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="11">
+        <v>101.37936149876001</v>
+      </c>
+      <c r="I19" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>174</v>
       </c>
@@ -2348,11 +2415,14 @@
       <c r="G20" s="8">
         <v>107925</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="11">
+        <v>377.34061216559002</v>
+      </c>
+      <c r="I20" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>99</v>
       </c>
@@ -2374,11 +2444,14 @@
       <c r="G21" s="8">
         <v>115922</v>
       </c>
-      <c r="H21" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="11">
+        <v>54.785101830972003</v>
+      </c>
+      <c r="I21" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>143</v>
       </c>
@@ -2400,11 +2473,14 @@
       <c r="G22" s="8">
         <v>109921</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="11">
+        <v>95.9</v>
+      </c>
+      <c r="I22" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>168</v>
       </c>
@@ -2426,11 +2502,14 @@
       <c r="G23" s="8">
         <v>106496</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="11">
+        <v>172.37424491618</v>
+      </c>
+      <c r="I23" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>114</v>
       </c>
@@ -2452,11 +2531,14 @@
       <c r="G24" s="8">
         <v>118051</v>
       </c>
-      <c r="H24" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="11">
+        <v>32666.202795237001</v>
+      </c>
+      <c r="I24" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>298</v>
       </c>
@@ -2478,11 +2560,14 @@
       <c r="G25" s="8">
         <v>109290</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="11">
+        <v>265.5</v>
+      </c>
+      <c r="I25" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>232</v>
       </c>
@@ -2504,11 +2589,14 @@
       <c r="G26" s="8">
         <v>95912</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="11">
+        <v>312.26314223983002</v>
+      </c>
+      <c r="I26" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>135</v>
       </c>
@@ -2530,11 +2618,14 @@
       <c r="G27" s="8">
         <v>108201</v>
       </c>
-      <c r="H27" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="11">
+        <v>6304.2826867164003</v>
+      </c>
+      <c r="I27" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>178</v>
       </c>
@@ -2556,11 +2647,14 @@
       <c r="G28" s="8">
         <v>103242</v>
       </c>
-      <c r="H28" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="11">
+        <v>90898.086033749001</v>
+      </c>
+      <c r="I28" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>270</v>
       </c>
@@ -2582,14 +2676,17 @@
       <c r="G29" s="8">
         <v>113726</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="11">
+        <v>2466.5</v>
+      </c>
+      <c r="I29" t="s">
         <v>359</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>151</v>
       </c>
@@ -2611,11 +2708,14 @@
       <c r="G30" s="8">
         <v>113073</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="11">
+        <v>125.94218267578999</v>
+      </c>
+      <c r="I30" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>189</v>
       </c>
@@ -2637,11 +2737,14 @@
       <c r="G31" s="8">
         <v>106307</v>
       </c>
-      <c r="H31" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="11">
+        <v>65.790000000000006</v>
+      </c>
+      <c r="I31" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>314</v>
       </c>
@@ -2663,14 +2766,17 @@
       <c r="G32" s="8">
         <v>73522</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="11">
+        <v>292.26491838587998</v>
+      </c>
+      <c r="I32" t="s">
         <v>356</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>208</v>
       </c>
@@ -2692,14 +2798,17 @@
       <c r="G33" s="8">
         <v>106942</v>
       </c>
-      <c r="H33" t="s">
-        <v>358</v>
+      <c r="H33" s="11">
+        <v>93.822495529487995</v>
       </c>
       <c r="I33" t="s">
+        <v>358</v>
+      </c>
+      <c r="J33" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>163</v>
       </c>
@@ -2721,14 +2830,17 @@
       <c r="G34" s="8">
         <v>111836</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="11">
+        <v>60.6</v>
+      </c>
+      <c r="I34" t="s">
         <v>356</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>73</v>
       </c>
@@ -2750,11 +2862,14 @@
       <c r="G35" s="8">
         <v>113257</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="11">
+        <v>5441.65</v>
+      </c>
+      <c r="I35" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>193</v>
       </c>
@@ -2776,11 +2891,14 @@
       <c r="G36" s="8">
         <v>110626</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="11">
+        <v>773.2</v>
+      </c>
+      <c r="I36" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>12</v>
       </c>
@@ -2802,14 +2920,17 @@
       <c r="G37" s="8">
         <v>99199</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="11">
+        <v>179.89785250451001</v>
+      </c>
+      <c r="I37" t="s">
         <v>356</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>79</v>
       </c>
@@ -2831,11 +2952,14 @@
       <c r="G38" s="8">
         <v>124211</v>
       </c>
-      <c r="H38" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H38" s="11">
+        <v>7296.1359495466004</v>
+      </c>
+      <c r="I38" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
@@ -2857,11 +2981,14 @@
       <c r="G39" s="8">
         <v>115571</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="11">
+        <v>518.77552559697995</v>
+      </c>
+      <c r="I39" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>133</v>
       </c>
@@ -2883,11 +3010,14 @@
       <c r="G40" s="8">
         <v>100880</v>
       </c>
-      <c r="H40" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H40" s="11">
+        <v>97.821263111883994</v>
+      </c>
+      <c r="I40" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
@@ -2909,14 +3039,17 @@
       <c r="G41" s="8">
         <v>104915</v>
       </c>
-      <c r="H41" t="s">
-        <v>358</v>
+      <c r="H41" s="11">
+        <v>14630.465763398999</v>
       </c>
       <c r="I41" t="s">
+        <v>358</v>
+      </c>
+      <c r="J41" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>280</v>
       </c>
@@ -2938,11 +3071,14 @@
       <c r="G42" s="8">
         <v>108083</v>
       </c>
-      <c r="H42" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H42" s="11">
+        <v>79.760000000000005</v>
+      </c>
+      <c r="I42" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>92</v>
       </c>
@@ -2964,14 +3100,17 @@
       <c r="G43" s="8">
         <v>108328</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="11">
+        <v>724.27560007953002</v>
+      </c>
+      <c r="I43" t="s">
         <v>359</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>197</v>
       </c>
@@ -2993,11 +3132,14 @@
       <c r="G44" s="8">
         <v>117187</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="11">
+        <v>787.16957975241996</v>
+      </c>
+      <c r="I44" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>214</v>
       </c>
@@ -3019,11 +3161,14 @@
       <c r="G45" s="8">
         <v>111095</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="11">
+        <v>152.84</v>
+      </c>
+      <c r="I45" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>247</v>
       </c>
@@ -3045,11 +3190,14 @@
       <c r="G46" s="8">
         <v>98118</v>
       </c>
-      <c r="H46" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H46" s="11">
+        <v>1629857.7169997001</v>
+      </c>
+      <c r="I46" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>167</v>
       </c>
@@ -3071,11 +3219,14 @@
       <c r="G47" s="8">
         <v>114003</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="11">
+        <v>41617.111439560998</v>
+      </c>
+      <c r="I47" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>253</v>
       </c>
@@ -3097,11 +3248,14 @@
       <c r="G48" s="8">
         <v>114717</v>
       </c>
-      <c r="H48" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H48" s="11">
+        <v>387.39978138316002</v>
+      </c>
+      <c r="I48" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>220</v>
       </c>
@@ -3123,11 +3277,14 @@
       <c r="G49" s="8">
         <v>114934</v>
       </c>
-      <c r="H49" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H49" s="11">
+        <v>1004.1651003599</v>
+      </c>
+      <c r="I49" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>185</v>
       </c>
@@ -3149,11 +3306,14 @@
       <c r="G50" s="8">
         <v>115636</v>
       </c>
-      <c r="H50" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H50" s="11">
+        <v>126590.00812</v>
+      </c>
+      <c r="I50" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>182</v>
       </c>
@@ -3175,11 +3335,14 @@
       <c r="G51" s="8">
         <v>96795</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="11">
+        <v>238.21212177807001</v>
+      </c>
+      <c r="I51" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>304</v>
       </c>
@@ -3201,11 +3364,14 @@
       <c r="G52" s="8">
         <v>113503</v>
       </c>
-      <c r="H52" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H52" s="11">
+        <v>1198.35759779</v>
+      </c>
+      <c r="I52" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>149</v>
       </c>
@@ -3227,11 +3393,14 @@
       <c r="G53" s="8">
         <v>111729</v>
       </c>
-      <c r="H53" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H53" s="11">
+        <v>871.11</v>
+      </c>
+      <c r="I53" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>224</v>
       </c>
@@ -3253,11 +3422,14 @@
       <c r="G54" s="8">
         <v>103383</v>
       </c>
-      <c r="H54" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H54" s="11">
+        <v>132829.46341296</v>
+      </c>
+      <c r="I54" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>300</v>
       </c>
@@ -3279,11 +3451,14 @@
       <c r="G55" s="8">
         <v>108733</v>
       </c>
-      <c r="H55" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H55" s="11">
+        <v>417.68744101790003</v>
+      </c>
+      <c r="I55" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>191</v>
       </c>
@@ -3305,11 +3480,14 @@
       <c r="G56" s="8">
         <v>105390</v>
       </c>
-      <c r="H56" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H56" s="11">
+        <v>11071.808585399</v>
+      </c>
+      <c r="I56" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>140</v>
       </c>
@@ -3331,11 +3509,14 @@
       <c r="G57" s="8">
         <v>107182</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H57" s="11">
+        <v>60.354185622050998</v>
+      </c>
+      <c r="I57" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>77</v>
       </c>
@@ -3357,11 +3538,14 @@
       <c r="G58" s="8">
         <v>76790</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H58" s="11">
+        <v>10009.231125931999</v>
+      </c>
+      <c r="I58" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>212</v>
       </c>
@@ -3383,11 +3567,14 @@
       <c r="G59" s="8">
         <v>109908</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H59" s="11">
+        <v>106.23</v>
+      </c>
+      <c r="I59" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>316</v>
       </c>
@@ -3409,11 +3596,14 @@
       <c r="G60" s="8">
         <v>106817</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H60" s="11">
+        <v>196.29688468201999</v>
+      </c>
+      <c r="I60" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>306</v>
       </c>
@@ -3435,11 +3625,14 @@
       <c r="G61" s="8">
         <v>112012</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="11">
+        <v>124.62</v>
+      </c>
+      <c r="I61" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>238</v>
       </c>
@@ -3461,11 +3654,14 @@
       <c r="G62" s="8">
         <v>122936</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H62" s="11">
+        <v>6341.7001184381998</v>
+      </c>
+      <c r="I62" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>60</v>
       </c>
@@ -3487,11 +3683,14 @@
       <c r="G63" s="8">
         <v>111487</v>
       </c>
-      <c r="H63" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H63" s="11">
+        <v>33182.269999999997</v>
+      </c>
+      <c r="I63" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>319</v>
       </c>
@@ -3513,14 +3712,17 @@
       <c r="G64" s="8">
         <v>109177</v>
       </c>
-      <c r="H64" t="s">
-        <v>358</v>
+      <c r="H64" s="11">
+        <v>50.66</v>
       </c>
       <c r="I64" t="s">
+        <v>358</v>
+      </c>
+      <c r="J64" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>222</v>
       </c>
@@ -3542,11 +3744,14 @@
       <c r="G65" s="8">
         <v>112182</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H65" s="11">
+        <v>540.86</v>
+      </c>
+      <c r="I65" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>0</v>
       </c>
@@ -3568,14 +3773,17 @@
       <c r="G66" s="8">
         <v>109490</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66" s="11">
+        <v>32.298701553755002</v>
+      </c>
+      <c r="I66" t="s">
         <v>356</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>255</v>
       </c>
@@ -3597,11 +3805,14 @@
       <c r="G67" s="8">
         <v>111833</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="11">
+        <v>81.348979801840002</v>
+      </c>
+      <c r="I67" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>249</v>
       </c>
@@ -3623,11 +3834,14 @@
       <c r="G68" s="8">
         <v>120783</v>
       </c>
-      <c r="H68" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H68" s="11">
+        <v>908595.6</v>
+      </c>
+      <c r="I68" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>49</v>
       </c>
@@ -3649,11 +3863,14 @@
       <c r="G69" s="8">
         <v>113021</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H69" s="11">
+        <v>53.912333026719999</v>
+      </c>
+      <c r="I69" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>203</v>
       </c>
@@ -3675,11 +3892,14 @@
       <c r="G70" s="8">
         <v>106368</v>
       </c>
-      <c r="H70" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H70" s="11">
+        <v>5585.8190134461001</v>
+      </c>
+      <c r="I70" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>323</v>
       </c>
@@ -3701,11 +3921,14 @@
       <c r="G71" s="8">
         <v>99250</v>
       </c>
-      <c r="H71" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H71" s="11">
+        <v>1192.4523421716001</v>
+      </c>
+      <c r="I71" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>292</v>
       </c>
@@ -3727,11 +3950,14 @@
       <c r="G72" s="8">
         <v>109334</v>
       </c>
-      <c r="H72" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H72" s="11">
+        <v>943.70171629073002</v>
+      </c>
+      <c r="I72" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>8</v>
       </c>
@@ -3753,14 +3979,17 @@
       <c r="G73" s="8">
         <v>111563</v>
       </c>
-      <c r="H73" t="s">
-        <v>358</v>
+      <c r="H73" s="11">
+        <v>41.85</v>
       </c>
       <c r="I73" t="s">
+        <v>358</v>
+      </c>
+      <c r="J73" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>45</v>
       </c>
@@ -3782,11 +4011,14 @@
       <c r="G74" s="8">
         <v>122975</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H74" s="11">
+        <v>122.42</v>
+      </c>
+      <c r="I74" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>240</v>
       </c>
@@ -3808,11 +4040,14 @@
       <c r="G75" s="8">
         <v>108583</v>
       </c>
-      <c r="H75" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H75" s="11">
+        <v>3818.4615529432999</v>
+      </c>
+      <c r="I75" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>52</v>
       </c>
@@ -3834,11 +4069,14 @@
       <c r="G76" s="8">
         <v>108954</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H76" s="11">
+        <v>266.45</v>
+      </c>
+      <c r="I76" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>226</v>
       </c>
@@ -3860,11 +4098,14 @@
       <c r="G77" s="8">
         <v>108111</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H77" s="11">
+        <v>83.07</v>
+      </c>
+      <c r="I77" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>165</v>
       </c>
@@ -3886,14 +4127,17 @@
       <c r="G78" s="8">
         <v>106096</v>
       </c>
-      <c r="H78" t="s">
-        <v>358</v>
+      <c r="H78" s="11">
+        <v>369.32581944304002</v>
       </c>
       <c r="I78" t="s">
+        <v>358</v>
+      </c>
+      <c r="J78" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>284</v>
       </c>
@@ -3915,11 +4159,14 @@
       <c r="G79" s="8">
         <v>116964</v>
       </c>
-      <c r="H79" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H79" s="11">
+        <v>17239.719430046</v>
+      </c>
+      <c r="I79" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>103</v>
       </c>
@@ -3941,11 +4188,14 @@
       <c r="G80" s="8">
         <v>121800</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H80" s="11">
+        <v>10639.861096371</v>
+      </c>
+      <c r="I80" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>130</v>
       </c>
@@ -3967,14 +4217,17 @@
       <c r="G81" s="8">
         <v>113262</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" s="11">
+        <v>29187.35</v>
+      </c>
+      <c r="I81" t="s">
         <v>356</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>89</v>
       </c>
@@ -3996,11 +4249,14 @@
       <c r="G82" s="8">
         <v>109258</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H82" s="11">
+        <v>155.83000000000001</v>
+      </c>
+      <c r="I82" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>294</v>
       </c>
@@ -4022,11 +4278,14 @@
       <c r="G83" s="8">
         <v>108255</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H83" s="11">
+        <v>104.41</v>
+      </c>
+      <c r="I83" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>159</v>
       </c>
@@ -4048,14 +4307,17 @@
       <c r="G84" s="8">
         <v>108551</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H84" s="11">
+        <v>567375.19810412999</v>
+      </c>
+      <c r="I84" t="s">
         <v>359</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>290</v>
       </c>
@@ -4077,11 +4339,14 @@
       <c r="G85" s="8">
         <v>111236</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H85" s="11">
+        <v>91.027220546961004</v>
+      </c>
+      <c r="I85" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>251</v>
       </c>
@@ -4103,14 +4368,17 @@
       <c r="G86" s="8">
         <v>119115</v>
       </c>
-      <c r="H86" t="s">
+      <c r="H86" s="11">
+        <v>165.67</v>
+      </c>
+      <c r="I86" t="s">
         <v>359</v>
       </c>
-      <c r="I86" t="s">
+      <c r="J86" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>112</v>
       </c>
@@ -4132,11 +4400,14 @@
       <c r="G87" s="8">
         <v>108799</v>
       </c>
-      <c r="H87" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H87" s="11">
+        <v>55.89</v>
+      </c>
+      <c r="I87" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>321</v>
       </c>
@@ -4158,11 +4429,14 @@
       <c r="G88" s="8">
         <v>113193</v>
       </c>
-      <c r="H88" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H88" s="11">
+        <v>748.13</v>
+      </c>
+      <c r="I88" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>257</v>
       </c>
@@ -4184,11 +4458,14 @@
       <c r="G89" s="8">
         <v>108797</v>
       </c>
-      <c r="H89" t="s">
+      <c r="H89" s="11">
+        <v>493.6</v>
+      </c>
+      <c r="I89" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>97</v>
       </c>
@@ -4210,11 +4487,14 @@
       <c r="G90" s="8">
         <v>110220</v>
       </c>
-      <c r="H90" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H90" s="11">
+        <v>148559.30332988</v>
+      </c>
+      <c r="I90" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>310</v>
       </c>
@@ -4236,11 +4516,14 @@
       <c r="G91" s="8">
         <v>108716</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H91" s="11">
+        <v>140.73481940635</v>
+      </c>
+      <c r="I91" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>201</v>
       </c>
@@ -4262,11 +4545,14 @@
       <c r="G92" s="8">
         <v>119328</v>
       </c>
-      <c r="H92" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H92" s="11">
+        <v>339.03662835054001</v>
+      </c>
+      <c r="I92" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>272</v>
       </c>
@@ -4288,11 +4574,14 @@
       <c r="G93" s="8">
         <v>72050</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H93" s="11">
+        <v>1348157.94</v>
+      </c>
+      <c r="I93" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>325</v>
       </c>
@@ -4314,11 +4603,14 @@
       <c r="G94" s="8">
         <v>116015</v>
       </c>
-      <c r="H94" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H94" s="11">
+        <v>1236.8250988090999</v>
+      </c>
+      <c r="I94" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>120</v>
       </c>
@@ -4340,11 +4632,14 @@
       <c r="G95" s="8">
         <v>119197</v>
       </c>
-      <c r="H95" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H95" s="11">
+        <v>16099.473298557999</v>
+      </c>
+      <c r="I95" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>205</v>
       </c>
@@ -4366,11 +4661,14 @@
       <c r="G96" s="8">
         <v>80402</v>
       </c>
-      <c r="H96" t="s">
+      <c r="H96" s="11">
+        <v>35721.830094308003</v>
+      </c>
+      <c r="I96" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>110</v>
       </c>
@@ -4392,14 +4690,17 @@
       <c r="G97" s="8">
         <v>120671</v>
       </c>
-      <c r="H97" t="s">
+      <c r="H97" s="11">
+        <v>362.76022332351999</v>
+      </c>
+      <c r="I97" t="s">
         <v>359</v>
       </c>
-      <c r="I97" t="s">
+      <c r="J97" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>101</v>
       </c>
@@ -4421,14 +4722,17 @@
       <c r="G98" s="8">
         <v>110831</v>
       </c>
-      <c r="H98" t="s">
-        <v>358</v>
+      <c r="H98" s="11">
+        <v>233.24485996496</v>
       </c>
       <c r="I98" t="s">
+        <v>358</v>
+      </c>
+      <c r="J98" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>43</v>
       </c>
@@ -4450,14 +4754,17 @@
       <c r="G99" s="8">
         <v>114115</v>
       </c>
-      <c r="H99" t="s">
+      <c r="H99" s="11">
+        <v>41.21</v>
+      </c>
+      <c r="I99" t="s">
         <v>356</v>
       </c>
-      <c r="I99" t="s">
+      <c r="J99" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>288</v>
       </c>
@@ -4479,11 +4786,14 @@
       <c r="G100" s="8">
         <v>107625</v>
       </c>
-      <c r="H100" t="s">
+      <c r="H100" s="11">
+        <v>4373.9920819497002</v>
+      </c>
+      <c r="I100" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>327</v>
       </c>
@@ -4505,11 +4815,14 @@
       <c r="G101" s="8">
         <v>120001</v>
       </c>
-      <c r="H101" t="s">
+      <c r="H101" s="11">
+        <v>162.4</v>
+      </c>
+      <c r="I101" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>308</v>
       </c>
@@ -4531,11 +4844,14 @@
       <c r="G102" s="8">
         <v>113823</v>
       </c>
-      <c r="H102" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H102" s="11">
+        <v>81962.210000000006</v>
+      </c>
+      <c r="I102" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>187</v>
       </c>
@@ -4557,14 +4873,17 @@
       <c r="G103" s="8">
         <v>105330</v>
       </c>
-      <c r="H103" t="s">
-        <v>358</v>
+      <c r="H103" s="11">
+        <v>729896.59069104004</v>
       </c>
       <c r="I103" t="s">
+        <v>358</v>
+      </c>
+      <c r="J103" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>264</v>
       </c>
@@ -4586,14 +4905,17 @@
       <c r="G104" s="8">
         <v>113312</v>
       </c>
-      <c r="H104" t="s">
+      <c r="H104" s="11">
+        <v>64.150000000000006</v>
+      </c>
+      <c r="I104" t="s">
         <v>359</v>
       </c>
-      <c r="I104" t="s">
+      <c r="J104" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>259</v>
       </c>
@@ -4615,14 +4937,17 @@
       <c r="G105" s="8">
         <v>123494</v>
       </c>
-      <c r="H105" t="s">
+      <c r="H105" s="11">
+        <v>9135.1200000000008</v>
+      </c>
+      <c r="I105" t="s">
         <v>356</v>
       </c>
-      <c r="I105" t="s">
+      <c r="J105" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>207</v>
       </c>
@@ -4644,11 +4969,14 @@
       <c r="G106" s="8">
         <v>109301</v>
       </c>
-      <c r="H106" t="s">
+      <c r="H106" s="11">
+        <v>2670.65</v>
+      </c>
+      <c r="I106" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>34</v>
       </c>
@@ -4670,11 +4998,14 @@
       <c r="G107" s="8">
         <v>106969</v>
       </c>
-      <c r="H107" t="s">
+      <c r="H107" s="11">
+        <v>168.41690660501001</v>
+      </c>
+      <c r="I107" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>16</v>
       </c>
@@ -4696,11 +5027,14 @@
       <c r="G108" s="8">
         <v>109426</v>
       </c>
-      <c r="H108" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H108" s="11">
+        <v>229.41644979851</v>
+      </c>
+      <c r="I108" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>26</v>
       </c>
@@ -4722,14 +5056,17 @@
       <c r="G109" s="8">
         <v>108064</v>
       </c>
-      <c r="H109" t="s">
+      <c r="H109" s="11">
+        <v>40.46</v>
+      </c>
+      <c r="I109" t="s">
         <v>356</v>
       </c>
-      <c r="I109" t="s">
+      <c r="J109" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>20</v>
       </c>
@@ -4751,11 +5088,14 @@
       <c r="G110" s="8">
         <v>108306</v>
       </c>
-      <c r="H110" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H110" s="11">
+        <v>184.73</v>
+      </c>
+      <c r="I110" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>138</v>
       </c>
@@ -4777,11 +5117,14 @@
       <c r="G111" s="8">
         <v>111522</v>
       </c>
-      <c r="H111" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H111" s="11">
+        <v>101.06674490261</v>
+      </c>
+      <c r="I111" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>35</v>
       </c>
@@ -4803,11 +5146,14 @@
       <c r="G112" s="8">
         <v>113634</v>
       </c>
-      <c r="H112" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H112" s="11">
+        <v>8879.3700000000008</v>
+      </c>
+      <c r="I112" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>29</v>
       </c>
@@ -4829,14 +5175,17 @@
       <c r="G113" s="8">
         <v>111823</v>
       </c>
-      <c r="H113" t="s">
-        <v>358</v>
+      <c r="H113" s="11">
+        <v>99.922918387364007</v>
       </c>
       <c r="I113" t="s">
+        <v>358</v>
+      </c>
+      <c r="J113" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>122</v>
       </c>
@@ -4858,11 +5207,14 @@
       <c r="G114" s="8">
         <v>101624</v>
       </c>
-      <c r="H114" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H114" s="11">
+        <v>90.051131839836003</v>
+      </c>
+      <c r="I114" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>236</v>
       </c>
@@ -4884,11 +5236,14 @@
       <c r="G115" s="8">
         <v>103607</v>
       </c>
-      <c r="H115" t="s">
+      <c r="H115" s="11">
+        <v>107.85800249306</v>
+      </c>
+      <c r="I115" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>157</v>
       </c>
@@ -4910,14 +5265,17 @@
       <c r="G116" s="8">
         <v>111841</v>
       </c>
-      <c r="H116" t="s">
-        <v>358</v>
+      <c r="H116" s="11">
+        <v>66394.207326479998</v>
       </c>
       <c r="I116" t="s">
+        <v>358</v>
+      </c>
+      <c r="J116" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>71</v>
       </c>
@@ -4939,11 +5297,14 @@
       <c r="G117" s="8">
         <v>117711</v>
       </c>
-      <c r="H117" t="s">
+      <c r="H117" s="11">
+        <v>170.78396268789001</v>
+      </c>
+      <c r="I117" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>91</v>
       </c>
@@ -4965,11 +5326,14 @@
       <c r="G118" s="8">
         <v>111805</v>
       </c>
-      <c r="H118" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H118" s="11">
+        <v>14768.97</v>
+      </c>
+      <c r="I118" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>329</v>
       </c>
@@ -4991,14 +5355,17 @@
       <c r="G119" s="8">
         <v>109650</v>
       </c>
-      <c r="H119" t="s">
-        <v>358</v>
+      <c r="H119" s="11">
+        <v>52.820341591442002</v>
       </c>
       <c r="I119" t="s">
+        <v>358</v>
+      </c>
+      <c r="J119" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>318</v>
       </c>
@@ -5020,11 +5387,14 @@
       <c r="G120" s="8">
         <v>101786</v>
       </c>
-      <c r="H120" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H120" s="11">
+        <v>868575.99819074001</v>
+      </c>
+      <c r="I120" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>87</v>
       </c>
@@ -5046,11 +5416,14 @@
       <c r="G121" s="8">
         <v>105333</v>
       </c>
-      <c r="H121" t="s">
+      <c r="H121" s="11">
+        <v>156.84952567884</v>
+      </c>
+      <c r="I121" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>145</v>
       </c>
@@ -5072,11 +5445,14 @@
       <c r="G122" s="8">
         <v>122839</v>
       </c>
-      <c r="H122" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H122" s="11">
+        <v>19342.197652207</v>
+      </c>
+      <c r="I122" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>85</v>
       </c>
@@ -5098,11 +5474,14 @@
       <c r="G123" s="8">
         <v>109112</v>
       </c>
-      <c r="H123" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H123" s="11">
+        <v>393412.85420226998</v>
+      </c>
+      <c r="I123" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>228</v>
       </c>
@@ -5124,11 +5503,14 @@
       <c r="G124" s="8">
         <v>103152</v>
       </c>
-      <c r="H124" t="s">
+      <c r="H124" s="11">
+        <v>56.770103353205997</v>
+      </c>
+      <c r="I124" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>282</v>
       </c>
@@ -5150,11 +5532,14 @@
       <c r="G125" s="8">
         <v>123040</v>
       </c>
-      <c r="H125" t="s">
+      <c r="H125" s="11">
+        <v>1123.4911766664</v>
+      </c>
+      <c r="I125" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>245</v>
       </c>
@@ -5176,11 +5561,14 @@
       <c r="G126" s="8">
         <v>121480</v>
       </c>
-      <c r="H126" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H126" s="11">
+        <v>13250.093994520999</v>
+      </c>
+      <c r="I126" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>124</v>
       </c>
@@ -5202,14 +5590,17 @@
       <c r="G127" s="8">
         <v>102420</v>
       </c>
-      <c r="H127" t="s">
+      <c r="H127" s="11">
+        <v>80.395633534249001</v>
+      </c>
+      <c r="I127" t="s">
         <v>359</v>
       </c>
-      <c r="I127" t="s">
+      <c r="J127" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>147</v>
       </c>
@@ -5231,11 +5622,14 @@
       <c r="G128" s="8">
         <v>116076</v>
       </c>
-      <c r="H128" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H128" s="11">
+        <v>148.66558843655</v>
+      </c>
+      <c r="I128" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>55</v>
       </c>
@@ -5257,11 +5651,14 @@
       <c r="G129" s="8">
         <v>103802</v>
       </c>
-      <c r="H129" t="s">
+      <c r="H129" s="11">
+        <v>131.05228508217999</v>
+      </c>
+      <c r="I129" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>195</v>
       </c>
@@ -5283,11 +5680,14 @@
       <c r="G130" s="8">
         <v>109500</v>
       </c>
-      <c r="H130" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H130" s="11">
+        <v>55.106740631561003</v>
+      </c>
+      <c r="I130" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>95</v>
       </c>
@@ -5309,11 +5709,14 @@
       <c r="G131" s="8">
         <v>119329</v>
       </c>
-      <c r="H131" t="s">
+      <c r="H131" s="11">
+        <v>2147.5733760285998</v>
+      </c>
+      <c r="I131" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>199</v>
       </c>
@@ -5335,11 +5738,14 @@
       <c r="G132" s="8">
         <v>113591</v>
       </c>
-      <c r="H132" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H132" s="11">
+        <v>48988.422154114</v>
+      </c>
+      <c r="I132" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>312</v>
       </c>
@@ -5361,11 +5767,14 @@
       <c r="G133" s="8">
         <v>110977</v>
       </c>
-      <c r="H133" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H133" s="11">
+        <v>980.03104091367004</v>
+      </c>
+      <c r="I133" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>266</v>
       </c>
@@ -5387,11 +5796,14 @@
       <c r="G134" s="8">
         <v>106398</v>
       </c>
-      <c r="H134" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H134" s="11">
+        <v>365.80196190624002</v>
+      </c>
+      <c r="I134" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>118</v>
       </c>
@@ -5413,14 +5825,17 @@
       <c r="G135" s="8">
         <v>106067</v>
       </c>
-      <c r="H135" t="s">
+      <c r="H135" s="11">
+        <v>116.28</v>
+      </c>
+      <c r="I135" t="s">
         <v>359</v>
       </c>
-      <c r="I135" t="s">
+      <c r="J135" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>83</v>
       </c>
@@ -5442,11 +5857,14 @@
       <c r="G136" s="8">
         <v>113639</v>
       </c>
-      <c r="H136" t="s">
+      <c r="H136" s="11">
+        <v>264.71447124779002</v>
+      </c>
+      <c r="I136" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>127</v>
       </c>
@@ -5468,11 +5886,14 @@
       <c r="G137" s="8">
         <v>68413</v>
       </c>
-      <c r="H137" t="s">
+      <c r="H137" s="11">
+        <v>190.61</v>
+      </c>
+      <c r="I137" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>58</v>
       </c>
@@ -5494,11 +5915,14 @@
       <c r="G138" s="8">
         <v>120105</v>
       </c>
-      <c r="H138" t="s">
+      <c r="H138" s="11">
+        <v>532.15</v>
+      </c>
+      <c r="I138" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>81</v>
       </c>
@@ -5520,11 +5944,14 @@
       <c r="G139" s="8">
         <v>101725</v>
       </c>
-      <c r="H139" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H139" s="11">
+        <v>74.147083660318003</v>
+      </c>
+      <c r="I139" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>278</v>
       </c>
@@ -5546,11 +5973,14 @@
       <c r="G140" s="8">
         <v>124287</v>
       </c>
-      <c r="H140" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H140" s="11">
+        <v>97.75</v>
+      </c>
+      <c r="I140" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>153</v>
       </c>
@@ -5572,11 +6002,14 @@
       <c r="G141" s="8">
         <v>101469</v>
       </c>
-      <c r="H141" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H141" s="11">
+        <v>133.88594130483</v>
+      </c>
+      <c r="I141" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>242</v>
       </c>
@@ -5598,14 +6031,17 @@
       <c r="G142" s="8">
         <v>114293</v>
       </c>
-      <c r="H142" t="s">
+      <c r="H142" s="11">
+        <v>43.987546041942998</v>
+      </c>
+      <c r="I142" t="s">
         <v>359</v>
       </c>
-      <c r="I142" t="s">
+      <c r="J142" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>210</v>
       </c>
@@ -5627,11 +6063,14 @@
       <c r="G143" s="8">
         <v>94495</v>
       </c>
-      <c r="H143" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H143" s="11">
+        <v>83.092372117186997</v>
+      </c>
+      <c r="I143" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>286</v>
       </c>
@@ -5653,11 +6092,14 @@
       <c r="G144" s="8">
         <v>115077</v>
       </c>
-      <c r="H144" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H144" s="11">
+        <v>33419.730000000003</v>
+      </c>
+      <c r="I144" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
         <v>276</v>
       </c>
@@ -5679,14 +6121,17 @@
       <c r="G145" s="8">
         <v>104735</v>
       </c>
-      <c r="H145" t="s">
+      <c r="H145" s="11">
+        <v>68.228120360877</v>
+      </c>
+      <c r="I145" t="s">
         <v>356</v>
       </c>
-      <c r="I145" t="s">
+      <c r="J145" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>39</v>
       </c>
@@ -5708,11 +6153,14 @@
       <c r="G146" s="8">
         <v>108227</v>
       </c>
-      <c r="H146" t="s">
+      <c r="H146" s="11">
+        <v>47.483262096274998</v>
+      </c>
+      <c r="I146" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>262</v>
       </c>
@@ -5734,14 +6182,17 @@
       <c r="G147" s="8">
         <v>103496</v>
       </c>
-      <c r="H147" t="s">
-        <v>358</v>
+      <c r="H147" s="11">
+        <v>37.652062892144002</v>
       </c>
       <c r="I147" t="s">
+        <v>358</v>
+      </c>
+      <c r="J147" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>274</v>
       </c>
@@ -5763,11 +6214,14 @@
       <c r="G148" s="8">
         <v>118303</v>
       </c>
-      <c r="H148" t="s">
+      <c r="H148" s="11">
+        <v>171.61810774423</v>
+      </c>
+      <c r="I148" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>155</v>
       </c>
@@ -5789,11 +6243,14 @@
       <c r="G149" s="8">
         <v>118778</v>
       </c>
-      <c r="H149" t="s">
+      <c r="H149" s="11">
+        <v>1330.8387375100001</v>
+      </c>
+      <c r="I149" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>218</v>
       </c>
@@ -5815,11 +6272,14 @@
       <c r="G150" s="8">
         <v>107910</v>
       </c>
-      <c r="H150" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H150" s="11">
+        <v>14226.664950486</v>
+      </c>
+      <c r="I150" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>170</v>
       </c>
@@ -5841,11 +6301,14 @@
       <c r="G151" s="8">
         <v>111237</v>
       </c>
-      <c r="H151" t="s">
+      <c r="H151" s="11">
+        <v>46.95</v>
+      </c>
+      <c r="I151" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>37</v>
       </c>
@@ -5867,12 +6330,15 @@
       <c r="G152" s="8">
         <v>113013</v>
       </c>
-      <c r="H152" t="s">
+      <c r="H152" s="11">
+        <v>7576.9828137132999</v>
+      </c>
+      <c r="I152" t="s">
         <v>358</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H152" xr:uid="{28BBEE73-48DC-47CC-ADDC-90B20223371E}"/>
+  <autoFilter ref="A1:I152" xr:uid="{28BBEE73-48DC-47CC-ADDC-90B20223371E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F152">
     <sortCondition ref="C2:C152"/>
   </sortState>
@@ -6302,5 +6768,6 @@
     <hyperlink ref="C119" r:id="rId423" tooltip="Division of North Sydney" display="https://en.wikipedia.org/wiki/Division_of_North_Sydney" xr:uid="{2A4BE194-FF6C-4C8A-B387-43F432E393E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId424"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with latest Lib/Nat statements on climate
</commit_message>
<xml_diff>
--- a/data/Representatives.xlsx
+++ b/data/Representatives.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Govt Climate Denialists\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F1DF10-CA04-4E7A-B4C6-E880BFB46375}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D51D2E-DBC1-4052-8057-4D6EA3C9683F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40830" yWindow="915" windowWidth="28800" windowHeight="15435" xr2:uid="{62D81309-DA17-4AA3-9DB3-296B4017ED59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{62D81309-DA17-4AA3-9DB3-296B4017ED59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="380">
   <si>
     <t>Hon Anthony Albanese</t>
   </si>
@@ -1370,6 +1370,21 @@
   </si>
   <si>
     <t>Area SqKm</t>
+  </si>
+  <si>
+    <t>"constituents do not want more action on climate policy"</t>
+  </si>
+  <si>
+    <t>Has expressed support for embracing renewable technologies to cut emissions</t>
+  </si>
+  <si>
+    <t>Has rebuked his colleagues for denying the science of climate change, but history of voting otherwise</t>
+  </si>
+  <si>
+    <t>Has stated that the recent fires are not a warning about climate change - they are climate change, but voting history…</t>
+  </si>
+  <si>
+    <t>History of voting against other climate/environment measures, stated that recent fires are due to arsonists, not climate change</t>
   </si>
 </sst>
 </file>
@@ -1822,8 +1837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADEF58E-A175-4784-867D-6B850DC00D7C}">
   <dimension ref="A1:J152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="M139" sqref="M139"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,7 +2164,7 @@
         <v>336</v>
       </c>
       <c r="F11" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="8">
         <v>109661</v>
@@ -2159,6 +2174,9 @@
       </c>
       <c r="I11" t="s">
         <v>358</v>
+      </c>
+      <c r="J11" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2323,7 +2341,7 @@
         <v>33</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" s="8">
         <v>109745</v>
@@ -2333,6 +2351,9 @@
       </c>
       <c r="I17" t="s">
         <v>358</v>
+      </c>
+      <c r="J17" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3095,7 +3116,7 @@
         <v>94</v>
       </c>
       <c r="F43" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="8">
         <v>108328</v>
@@ -3107,7 +3128,7 @@
         <v>359</v>
       </c>
       <c r="J43" t="s">
-        <v>362</v>
+        <v>379</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4627,7 +4648,7 @@
         <v>57</v>
       </c>
       <c r="F95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G95" s="8">
         <v>119197</v>
@@ -4637,6 +4658,9 @@
       </c>
       <c r="I95" t="s">
         <v>358</v>
+      </c>
+      <c r="J95" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5675,7 +5699,7 @@
         <v>11</v>
       </c>
       <c r="F130">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G130" s="8">
         <v>109500</v>
@@ -5685,6 +5709,9 @@
       </c>
       <c r="I130" t="s">
         <v>358</v>
+      </c>
+      <c r="J130" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="131" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>